<commit_message>
Written tests for Excel table.
</commit_message>
<xml_diff>
--- a/excel_files/wines.xlsx
+++ b/excel_files/wines.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\devman\wine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\devman\wine\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,100 +21,100 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
+    <t>Белая леди</t>
+  </si>
+  <si>
+    <t>Дамский пальчик</t>
+  </si>
+  <si>
+    <t>belaya_ledi.png</t>
+  </si>
+  <si>
+    <t>Ркацители</t>
+  </si>
+  <si>
+    <t>rkaciteli.png</t>
+  </si>
+  <si>
+    <t>Хванчкара</t>
+  </si>
+  <si>
+    <t>Александраули</t>
+  </si>
+  <si>
+    <t>hvanchkara.png</t>
+  </si>
+  <si>
+    <t>Белые вина</t>
+  </si>
+  <si>
+    <t>Напитки</t>
+  </si>
+  <si>
+    <t>Коньяк классический</t>
+  </si>
+  <si>
+    <t>konyak_klassicheskyi.png</t>
+  </si>
+  <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Черный лекарь</t>
+  </si>
+  <si>
+    <t>Качич</t>
+  </si>
+  <si>
+    <t>chernyi_lekar.png</t>
+  </si>
+  <si>
+    <t>Кокур</t>
+  </si>
+  <si>
+    <t>kokur.png</t>
+  </si>
+  <si>
+    <t>Киндзмараули</t>
+  </si>
+  <si>
+    <t>Саперави</t>
+  </si>
+  <si>
+    <t>kindzmarauli.png</t>
+  </si>
+  <si>
+    <t>Чача</t>
+  </si>
+  <si>
+    <t>chacha.png</t>
+  </si>
+  <si>
+    <t>Коньяк кизиловый</t>
+  </si>
+  <si>
+    <t>konyak_kizilovyi.png</t>
+  </si>
+  <si>
+    <t>Выгодное предложение</t>
+  </si>
+  <si>
+    <t>Акция</t>
+  </si>
+  <si>
+    <t>Картинка</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Сорт</t>
+  </si>
+  <si>
     <t>Название</t>
   </si>
   <si>
-    <t>Сорт</t>
-  </si>
-  <si>
-    <t>Цена</t>
-  </si>
-  <si>
-    <t>Картинка</t>
-  </si>
-  <si>
-    <t>Белая леди</t>
-  </si>
-  <si>
-    <t>Дамский пальчик</t>
-  </si>
-  <si>
-    <t>belaya_ledi.png</t>
-  </si>
-  <si>
-    <t>Ркацители</t>
-  </si>
-  <si>
-    <t>rkaciteli.png</t>
-  </si>
-  <si>
-    <t>Хванчкара</t>
-  </si>
-  <si>
-    <t>Александраули</t>
-  </si>
-  <si>
-    <t>hvanchkara.png</t>
-  </si>
-  <si>
     <t>Категория</t>
-  </si>
-  <si>
-    <t>Белые вина</t>
-  </si>
-  <si>
-    <t>Напитки</t>
-  </si>
-  <si>
-    <t>Коньяк классический</t>
-  </si>
-  <si>
-    <t>konyak_klassicheskyi.png</t>
-  </si>
-  <si>
-    <t>Красные вина</t>
-  </si>
-  <si>
-    <t>Черный лекарь</t>
-  </si>
-  <si>
-    <t>Качич</t>
-  </si>
-  <si>
-    <t>chernyi_lekar.png</t>
-  </si>
-  <si>
-    <t>Кокур</t>
-  </si>
-  <si>
-    <t>kokur.png</t>
-  </si>
-  <si>
-    <t>Киндзмараули</t>
-  </si>
-  <si>
-    <t>Саперави</t>
-  </si>
-  <si>
-    <t>kindzmarauli.png</t>
-  </si>
-  <si>
-    <t>Чача</t>
-  </si>
-  <si>
-    <t>chacha.png</t>
-  </si>
-  <si>
-    <t>Коньяк кизиловый</t>
-  </si>
-  <si>
-    <t>konyak_kizilovyi.png</t>
-  </si>
-  <si>
-    <t>Акция</t>
-  </si>
-  <si>
-    <t>Выгодное предложение</t>
   </si>
 </sst>
 </file>
@@ -404,9 +404,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -420,181 +418,181 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <v>399</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4">
         <v>399</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4">
         <v>350</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5" s="4">
         <v>499</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4">
         <v>550</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4">
         <v>450</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4">
         <v>550</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4">
         <v>299</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
         <v>350</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F10" s="3"/>
     </row>

</xml_diff>